<commit_message>
removed cleaning on table sP1
</commit_message>
<xml_diff>
--- a/Output/TABLE_P1a.xlsx
+++ b/Output/TABLE_P1a.xlsx
@@ -132,22 +132,22 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>117.23352713178295</v>
+        <v>147.71975601491019</v>
       </c>
       <c r="C2">
-        <v>27.402790697674419</v>
+        <v>23.872162485065711</v>
       </c>
       <c r="D2">
-        <v>845.11639056310491</v>
+        <v>1063.504916237069</v>
       </c>
       <c r="E2">
-        <v>58.84816590112824</v>
+        <v>49.059182334552915</v>
       </c>
       <c r="F2">
-        <v>89.83073643410853</v>
+        <v>123.84759352984447</v>
       </c>
       <c r="G2">
-        <v>14.99032204705949</v>
+        <v>13.027148546919239</v>
       </c>
     </row>
     <row r="3">
@@ -155,22 +155,22 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>42093.114053144862</v>
+        <v>58150.946746828689</v>
       </c>
       <c r="C3">
-        <v>5164.5521969193433</v>
+        <v>3975.713398269937</v>
       </c>
       <c r="D3">
-        <v>637960.08323259384</v>
+        <v>759169.99574361613</v>
       </c>
       <c r="E3">
-        <v>11836.293976948939</v>
+        <v>10107.992072367198</v>
       </c>
       <c r="F3">
-        <v>36928.561856225519</v>
+        <v>54175.233348558751</v>
       </c>
       <c r="G3">
-        <v>11258.041421405749</v>
+        <v>9298.9184793956028</v>
       </c>
     </row>
     <row r="4">
@@ -178,22 +178,22 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>2971.6896928280821</v>
+        <v>3074.7134027941652</v>
       </c>
       <c r="C4">
-        <v>559.6127534014629</v>
+        <v>429.38602486757401</v>
       </c>
       <c r="D4">
-        <v>31644.906058286884</v>
+        <v>25037.785176689635</v>
       </c>
       <c r="E4">
-        <v>1993.7820574885916</v>
+        <v>1612.6354098410256</v>
       </c>
       <c r="F4">
-        <v>2412.076939426619</v>
+        <v>2645.327377926591</v>
       </c>
       <c r="G4">
-        <v>558.40925476974144</v>
+        <v>305.4960571882707</v>
       </c>
     </row>
     <row r="5">
@@ -201,22 +201,22 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>32775.917458201024</v>
+        <v>46125.585812180259</v>
       </c>
       <c r="C5">
-        <v>2492.2069140193134</v>
+        <v>2055.0905018921512</v>
       </c>
       <c r="D5">
-        <v>559054.1203955923</v>
+        <v>647590.91457900731</v>
       </c>
       <c r="E5">
-        <v>6656.7635073765041</v>
+        <v>6271.8004843207045</v>
       </c>
       <c r="F5">
-        <v>30283.710544181711</v>
+        <v>44070.495310288112</v>
       </c>
       <c r="G5">
-        <v>9933.7994812355137</v>
+        <v>8024.6705394324053</v>
       </c>
     </row>
     <row r="6">
@@ -224,22 +224,22 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>11981.933740890256</v>
+        <v>18257.890227933472</v>
       </c>
       <c r="C6">
-        <v>2797.1205799869172</v>
+        <v>2104.7503877541872</v>
       </c>
       <c r="D6">
-        <v>108844.18436135496</v>
+        <v>227306.12426804498</v>
       </c>
       <c r="E6">
-        <v>6071.2004786355892</v>
+        <v>4983.3053038042881</v>
       </c>
       <c r="F6">
-        <v>9184.8131609033389</v>
+        <v>16153.139840179285</v>
       </c>
       <c r="G6">
-        <v>1965.175885373458</v>
+        <v>2850.247103543787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>